<commit_message>
partial update. - UTS and Modulus
</commit_message>
<xml_diff>
--- a/BIRDSHOT-HEADATA-Alvi/Training-Modulus2/results0/model_predictions1.xlsx
+++ b/BIRDSHOT-HEADATA-Alvi/Training-Modulus2/results0/model_predictions1.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,7 +469,7 @@
         <v>199.57</v>
       </c>
       <c r="J2">
-        <v>192.6139221191406</v>
+        <v>193.5206604003906</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -501,7 +501,7 @@
         <v>190.55</v>
       </c>
       <c r="J3">
-        <v>192.7747344970703</v>
+        <v>189.0159149169922</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -533,7 +533,7 @@
         <v>161.94</v>
       </c>
       <c r="J4">
-        <v>171.2662200927734</v>
+        <v>157.2640991210938</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -565,7 +565,7 @@
         <v>203.53</v>
       </c>
       <c r="J5">
-        <v>197.6770629882812</v>
+        <v>202.7201690673828</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -597,7 +597,7 @@
         <v>171.74</v>
       </c>
       <c r="J6">
-        <v>161.8553314208984</v>
+        <v>171.2957000732422</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -629,7 +629,7 @@
         <v>173.17</v>
       </c>
       <c r="J7">
-        <v>169.1324462890625</v>
+        <v>169.0731506347656</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -661,7 +661,7 @@
         <v>200.47</v>
       </c>
       <c r="J8">
-        <v>196.5857696533203</v>
+        <v>196.3484191894531</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -693,7 +693,7 @@
         <v>194.27</v>
       </c>
       <c r="J9">
-        <v>193.2171630859375</v>
+        <v>200.0079040527344</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -725,7 +725,7 @@
         <v>162.1</v>
       </c>
       <c r="J10">
-        <v>178.6652221679688</v>
+        <v>164.6422424316406</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -757,71 +757,71 @@
         <v>207.26</v>
       </c>
       <c r="J11">
-        <v>196.9932403564453</v>
+        <v>202.7879791259766</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>212.65</v>
+        <v>180.09</v>
       </c>
       <c r="J12">
-        <v>208.5606231689453</v>
+        <v>179.9928894042969</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I13">
-        <v>182.8</v>
+        <v>212.65</v>
       </c>
       <c r="J13">
-        <v>183.0410003662109</v>
+        <v>205.2185821533203</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -829,63 +829,63 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>44.99999999999999</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="H14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>190.02</v>
+        <v>189.94</v>
       </c>
       <c r="J14">
-        <v>193.9942932128906</v>
+        <v>198.2015686035156</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>20</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>178.91</v>
+        <v>182.8</v>
       </c>
       <c r="J15">
-        <v>198.2785186767578</v>
+        <v>192.5529327392578</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -893,95 +893,95 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>44.99999999999999</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="H16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>212.4</v>
+        <v>190.02</v>
       </c>
       <c r="J16">
-        <v>208.9917755126953</v>
+        <v>198.6741485595703</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I17">
-        <v>170.22</v>
+        <v>178.91</v>
       </c>
       <c r="J17">
-        <v>176.0575866699219</v>
+        <v>187.6985015869141</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>54.99999999999999</v>
+        <v>75</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I18">
-        <v>209.96</v>
+        <v>212.4</v>
       </c>
       <c r="J18">
-        <v>193.8027801513672</v>
+        <v>208.8190765380859</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -989,63 +989,63 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>54.99999999999999</v>
+        <v>45</v>
       </c>
       <c r="H19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>205</v>
+        <v>170.22</v>
       </c>
       <c r="J19">
-        <v>208.7668762207031</v>
+        <v>172.1693725585938</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B20">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>35</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H20">
         <v>5</v>
       </c>
       <c r="I20">
-        <v>165.27</v>
+        <v>209.96</v>
       </c>
       <c r="J20">
-        <v>179.9722747802734</v>
+        <v>203.5467529296875</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1053,31 +1053,31 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>54.99999999999999</v>
+      </c>
+      <c r="H21">
         <v>25</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>45</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
       <c r="I21">
-        <v>174.64</v>
+        <v>205</v>
       </c>
       <c r="J21">
-        <v>179.4411010742188</v>
+        <v>199.2821502685547</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1085,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1100,144 +1100,144 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H22">
         <v>5</v>
       </c>
       <c r="I22">
-        <v>169.54</v>
+        <v>165.27</v>
       </c>
       <c r="J22">
-        <v>186.7634887695312</v>
+        <v>165.6304321289062</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H23">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>184.96</v>
+        <v>174.64</v>
       </c>
       <c r="J23">
-        <v>183.5744171142578</v>
+        <v>190.1134490966797</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F24">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I24">
-        <v>178.42</v>
+        <v>169.54</v>
       </c>
       <c r="J24">
-        <v>174.2621917724609</v>
+        <v>181.3739776611328</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G25">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H25">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I25">
-        <v>207.29</v>
+        <v>184.96</v>
       </c>
       <c r="J25">
-        <v>208.1166229248047</v>
+        <v>183.8725433349609</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <v>54.99999999999999</v>
+        <v>56</v>
       </c>
       <c r="H26">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I26">
-        <v>194.55</v>
+        <v>202.62</v>
       </c>
       <c r="J26">
-        <v>199.9582977294922</v>
+        <v>188.4308471679688</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1245,31 +1245,31 @@
         <v>4</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E27">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F27">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G27">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H27">
         <v>4</v>
       </c>
       <c r="I27">
-        <v>165.34</v>
+        <v>178.42</v>
       </c>
       <c r="J27">
-        <v>188.9590301513672</v>
+        <v>177.8637084960938</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1277,31 +1277,31 @@
         <v>0</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H28">
         <v>15</v>
       </c>
       <c r="I28">
-        <v>225</v>
+        <v>207.29</v>
       </c>
       <c r="J28">
-        <v>209.9421234130859</v>
+        <v>206.2197113037109</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1309,31 +1309,31 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="C29">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
       <c r="G29">
-        <v>10</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I29">
-        <v>237.14</v>
+        <v>194.55</v>
       </c>
       <c r="J29">
-        <v>221.3225860595703</v>
+        <v>194.4839019775391</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1341,31 +1341,31 @@
         <v>4</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>24</v>
+      </c>
+      <c r="F30">
         <v>12</v>
       </c>
-      <c r="E30">
-        <v>20</v>
-      </c>
-      <c r="F30">
-        <v>8</v>
-      </c>
       <c r="G30">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I30">
-        <v>189.5</v>
+        <v>165.34</v>
       </c>
       <c r="J30">
-        <v>176.1422729492188</v>
+        <v>179.9928894042969</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1373,31 +1373,31 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C31">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H31">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I31">
-        <v>209.59</v>
+        <v>225</v>
       </c>
       <c r="J31">
-        <v>207.7519226074219</v>
+        <v>217.3385162353516</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1405,95 +1405,95 @@
         <v>0</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I32">
-        <v>263.51</v>
+        <v>237.14</v>
       </c>
       <c r="J32">
-        <v>240.0944366455078</v>
+        <v>228.0111846923828</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E33">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G33">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H33">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>199.87</v>
+        <v>189.5</v>
       </c>
       <c r="J33">
-        <v>194.8812866210938</v>
+        <v>180.7701416015625</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F34">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I34">
-        <v>156.06</v>
+        <v>209.59</v>
       </c>
       <c r="J34">
-        <v>182.2429809570312</v>
+        <v>206.9410095214844</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1501,31 +1501,31 @@
         <v>0</v>
       </c>
       <c r="B35">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G35">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H35">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="I35">
-        <v>213.68</v>
+        <v>201.32</v>
       </c>
       <c r="J35">
-        <v>193.8992767333984</v>
+        <v>237.45068359375</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1536,28 +1536,28 @@
         <v>20</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G36">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H36">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I36">
-        <v>215</v>
+        <v>263.51</v>
       </c>
       <c r="J36">
-        <v>205.6905822753906</v>
+        <v>237.45068359375</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="B37">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -1574,86 +1574,86 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H37">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I37">
-        <v>202.06</v>
+        <v>199.87</v>
       </c>
       <c r="J37">
-        <v>198.4251098632812</v>
+        <v>199.3091888427734</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B38">
-        <v>35.00000000000001</v>
+        <v>12</v>
       </c>
       <c r="C38">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G38">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="H38">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I38">
-        <v>217.91</v>
+        <v>197.69</v>
       </c>
       <c r="J38">
-        <v>215.7884368896484</v>
+        <v>227.1830139160156</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>35.00000000000001</v>
+        <v>12</v>
       </c>
       <c r="C39">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G39">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H39">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I39">
-        <v>199.06</v>
+        <v>156.06</v>
       </c>
       <c r="J39">
-        <v>210.9718322753906</v>
+        <v>176.4345397949219</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="B40">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -1670,22 +1670,22 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="H40">
         <v>25</v>
       </c>
       <c r="I40">
-        <v>234.03</v>
+        <v>213.68</v>
       </c>
       <c r="J40">
-        <v>217.4901733398438</v>
+        <v>198.7969970703125</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1693,31 +1693,31 @@
         <v>0</v>
       </c>
       <c r="B41">
-        <v>44.99999999999999</v>
+        <v>20</v>
       </c>
       <c r="C41">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G41">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="H41">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I41">
-        <v>229.63</v>
+        <v>215</v>
       </c>
       <c r="J41">
-        <v>216.7311096191406</v>
+        <v>205.7451782226562</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1725,10 +1725,10 @@
         <v>0</v>
       </c>
       <c r="B42">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C42">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1740,16 +1740,16 @@
         <v>0</v>
       </c>
       <c r="G42">
+        <v>20</v>
+      </c>
+      <c r="H42">
         <v>30</v>
       </c>
-      <c r="H42">
-        <v>15</v>
-      </c>
       <c r="I42">
-        <v>193.22</v>
+        <v>202.06</v>
       </c>
       <c r="J42">
-        <v>204.0700378417969</v>
+        <v>202.6976318359375</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1757,63 +1757,63 @@
         <v>0</v>
       </c>
       <c r="B43">
-        <v>40</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H43">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I43">
-        <v>237.02</v>
+        <v>217.91</v>
       </c>
       <c r="J43">
-        <v>207.8111267089844</v>
+        <v>212.5868377685547</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B44">
-        <v>12</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D44">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F44">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I44">
-        <v>141.59</v>
+        <v>199.06</v>
       </c>
       <c r="J44">
-        <v>175.3040771484375</v>
+        <v>201.6929626464844</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1821,31 +1821,31 @@
         <v>0</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C45">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
+        <v>15</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>15</v>
+      </c>
+      <c r="H45">
         <v>25</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>50</v>
-      </c>
-      <c r="H45">
-        <v>5</v>
-      </c>
       <c r="I45">
-        <v>187.18</v>
+        <v>234.03</v>
       </c>
       <c r="J45">
-        <v>190.4759521484375</v>
+        <v>224.7321929931641</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1853,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="B46">
-        <v>35.00000000000001</v>
+        <v>44.99999999999999</v>
       </c>
       <c r="C46">
         <v>15</v>
@@ -1862,150 +1862,150 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H46">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I46">
-        <v>223.68</v>
+        <v>229.63</v>
       </c>
       <c r="J46">
-        <v>224.1782073974609</v>
+        <v>221.6792602539062</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B47">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C47">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E47">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G47">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H47">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I47">
-        <v>196.74</v>
+        <v>198.95</v>
       </c>
       <c r="J47">
-        <v>204.3441772460938</v>
+        <v>192.2540435791016</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F48">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H48">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I48">
-        <v>162.29</v>
+        <v>193.22</v>
       </c>
       <c r="J48">
-        <v>184.6997985839844</v>
+        <v>194.07275390625</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F49">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="H49">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="I49">
-        <v>191.23</v>
+        <v>237.02</v>
       </c>
       <c r="J49">
-        <v>202.8037261962891</v>
+        <v>229.406982421875</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E50">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G50">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I50">
-        <v>178.43</v>
+        <v>141.59</v>
       </c>
       <c r="J50">
-        <v>187.2025451660156</v>
+        <v>178.5405883789062</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2013,63 +2013,63 @@
         <v>0</v>
       </c>
       <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
         <v>25</v>
       </c>
-      <c r="C51">
-        <v>10</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>5</v>
-      </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H51">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I51">
-        <v>198.66</v>
+        <v>187.18</v>
       </c>
       <c r="J51">
-        <v>197.0372161865234</v>
+        <v>185.9449462890625</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B52">
-        <v>8</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C52">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F52">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I52">
-        <v>171.77</v>
+        <v>223.68</v>
       </c>
       <c r="J52">
-        <v>171.6454925537109</v>
+        <v>216.2131805419922</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2077,16 +2077,16 @@
         <v>0</v>
       </c>
       <c r="B53">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2095,45 +2095,45 @@
         <v>40</v>
       </c>
       <c r="H53">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I53">
-        <v>189.31</v>
+        <v>196.74</v>
       </c>
       <c r="J53">
-        <v>190.0306854248047</v>
+        <v>196.3951873779297</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E54">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G54">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>157.73</v>
+        <v>170.41</v>
       </c>
       <c r="J54">
-        <v>158.9559936523438</v>
+        <v>178.5405883789062</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2141,63 +2141,63 @@
         <v>0</v>
       </c>
       <c r="B55">
-        <v>44.99999999999999</v>
+        <v>12</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E55">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G55">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="H55">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I55">
-        <v>196.42</v>
+        <v>183.07</v>
       </c>
       <c r="J55">
-        <v>195.1272583007812</v>
+        <v>190.0183258056641</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B56">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E56">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G56">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H56">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I56">
-        <v>162.96</v>
+        <v>162.29</v>
       </c>
       <c r="J56">
-        <v>178.178466796875</v>
+        <v>170.241455078125</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2205,159 +2205,159 @@
         <v>4</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C57">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>4</v>
       </c>
       <c r="F57">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G57">
         <v>52</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I57">
-        <v>182.28</v>
+        <v>191.23</v>
       </c>
       <c r="J57">
-        <v>175.2132873535156</v>
+        <v>189.3750305175781</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B58">
-        <v>55.00000000000001</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G58">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="H58">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I58">
-        <v>197.23</v>
+        <v>181.2</v>
       </c>
       <c r="J58">
-        <v>192.9765930175781</v>
+        <v>185.4855804443359</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B59">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D59">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F59">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I59">
-        <v>229.87</v>
+        <v>178.43</v>
       </c>
       <c r="J59">
-        <v>207.88134765625</v>
+        <v>189.1533355712891</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B60">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C60">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F60">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H60">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I60">
-        <v>180.26</v>
+        <v>198.66</v>
       </c>
       <c r="J60">
-        <v>190.5270233154297</v>
+        <v>203.6840057373047</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B61">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E61">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G61">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H61">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I61">
-        <v>189.61</v>
+        <v>171.77</v>
       </c>
       <c r="J61">
-        <v>192.7213897705078</v>
+        <v>178.4182434082031</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2365,31 +2365,31 @@
         <v>0</v>
       </c>
       <c r="B62">
-        <v>35.00000000000001</v>
+        <v>25</v>
       </c>
       <c r="C62">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="G62">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H62">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I62">
-        <v>208.46</v>
+        <v>189.31</v>
       </c>
       <c r="J62">
-        <v>218.8370361328125</v>
+        <v>188.4877777099609</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2397,31 +2397,31 @@
         <v>0</v>
       </c>
       <c r="B63">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C63">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="G63">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="H63">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>219.29</v>
+        <v>157.73</v>
       </c>
       <c r="J63">
-        <v>216.4721527099609</v>
+        <v>151.4253997802734</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2429,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>44.99999999999999</v>
       </c>
       <c r="C64">
         <v>5</v>
@@ -2438,86 +2438,86 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F64">
         <v>0</v>
       </c>
       <c r="G64">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H64">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I64">
-        <v>211.23</v>
+        <v>196.42</v>
       </c>
       <c r="J64">
-        <v>200.2881927490234</v>
+        <v>196.0731964111328</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="F65">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I65">
-        <v>189.54</v>
+        <v>162.96</v>
       </c>
       <c r="J65">
-        <v>201.7102508544922</v>
+        <v>165.0841217041016</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E66">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G66">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H66">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I66">
-        <v>209.17</v>
+        <v>182.28</v>
       </c>
       <c r="J66">
-        <v>208.7992706298828</v>
+        <v>182.6378021240234</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2525,31 +2525,31 @@
         <v>0</v>
       </c>
       <c r="B67">
-        <v>4</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F67">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H67">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I67">
-        <v>199.98</v>
+        <v>197.23</v>
       </c>
       <c r="J67">
-        <v>202.1588134765625</v>
+        <v>203.0479888916016</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2557,63 +2557,63 @@
         <v>0</v>
       </c>
       <c r="B68">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C68">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E68">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G68">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H68">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I68">
-        <v>206.84</v>
+        <v>229.87</v>
       </c>
       <c r="J68">
-        <v>207.2539520263672</v>
+        <v>198.2015686035156</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B69">
         <v>12</v>
       </c>
       <c r="C69">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F69">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G69">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H69">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="I69">
-        <v>192.43</v>
+        <v>180.26</v>
       </c>
       <c r="J69">
-        <v>192.4772491455078</v>
+        <v>188.4308471679688</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2624,28 +2624,28 @@
         <v>30</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H70">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I70">
-        <v>188.44</v>
+        <v>189.61</v>
       </c>
       <c r="J70">
-        <v>185.75537109375</v>
+        <v>193.7273712158203</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2653,31 +2653,31 @@
         <v>0</v>
       </c>
       <c r="B71">
-        <v>20</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C71">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
       <c r="G71">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H71">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I71">
-        <v>207.91</v>
+        <v>208.46</v>
       </c>
       <c r="J71">
-        <v>201.9089202880859</v>
+        <v>208.8983306884766</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2685,31 +2685,31 @@
         <v>0</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C72">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F72">
         <v>0</v>
       </c>
       <c r="G72">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H72">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I72">
-        <v>202.88</v>
+        <v>219.29</v>
       </c>
       <c r="J72">
-        <v>204.9272155761719</v>
+        <v>204.5302124023438</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2717,95 +2717,95 @@
         <v>0</v>
       </c>
       <c r="B73">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C73">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H73">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I73">
-        <v>199.81</v>
+        <v>211.23</v>
       </c>
       <c r="J73">
-        <v>196.5753326416016</v>
+        <v>198.0908813476562</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B74">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C74">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E74">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G74">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="H74">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>203.35</v>
+        <v>189.54</v>
       </c>
       <c r="J74">
-        <v>208.9655609130859</v>
+        <v>193.2817993164062</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D75">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F75">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H75">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I75">
-        <v>234.5</v>
+        <v>209.17</v>
       </c>
       <c r="J75">
-        <v>212.1127471923828</v>
+        <v>203.5997619628906</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2813,31 +2813,31 @@
         <v>0</v>
       </c>
       <c r="B76">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C76">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E76">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G76">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H76">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I76">
-        <v>206.43</v>
+        <v>199.98</v>
       </c>
       <c r="J76">
-        <v>205.6038360595703</v>
+        <v>190.0374755859375</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2845,63 +2845,63 @@
         <v>0</v>
       </c>
       <c r="B77">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
       <c r="E77">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F77">
         <v>0</v>
       </c>
       <c r="G77">
-        <v>54.99999999999999</v>
+        <v>40</v>
       </c>
       <c r="H77">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I77">
-        <v>196.61</v>
+        <v>206.84</v>
       </c>
       <c r="J77">
-        <v>191.0798187255859</v>
+        <v>200.1914520263672</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
+        <v>4</v>
+      </c>
+      <c r="F78">
+        <v>16</v>
+      </c>
+      <c r="G78">
         <v>40</v>
       </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>45</v>
-      </c>
       <c r="H78">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="I78">
-        <v>211.67</v>
+        <v>192.43</v>
       </c>
       <c r="J78">
-        <v>204.4612579345703</v>
+        <v>185.7575988769531</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2909,16 +2909,16 @@
         <v>0</v>
       </c>
       <c r="B79">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C79">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -2930,42 +2930,42 @@
         <v>5</v>
       </c>
       <c r="I79">
-        <v>213.37</v>
+        <v>188.44</v>
       </c>
       <c r="J79">
-        <v>205.3970184326172</v>
+        <v>187.3595581054688</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B80">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D80">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G80">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H80">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="I80">
-        <v>179.43</v>
+        <v>207.91</v>
       </c>
       <c r="J80">
-        <v>184.7304534912109</v>
+        <v>206.3297119140625</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -2973,31 +2973,31 @@
         <v>0</v>
       </c>
       <c r="B81">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E81">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G81">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H81">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I81">
-        <v>213.93</v>
+        <v>187.31</v>
       </c>
       <c r="J81">
-        <v>208.0306091308594</v>
+        <v>205.67724609375</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3005,10 +3005,10 @@
         <v>0</v>
       </c>
       <c r="B82">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C82">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3020,16 +3020,16 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="H82">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I82">
-        <v>195.4</v>
+        <v>202.88</v>
       </c>
       <c r="J82">
-        <v>200.8869934082031</v>
+        <v>200.0972442626953</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3037,31 +3037,31 @@
         <v>0</v>
       </c>
       <c r="B83">
+        <v>20</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>5</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
         <v>40</v>
       </c>
-      <c r="C83">
+      <c r="H83">
         <v>25</v>
       </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>10</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-      <c r="G83">
-        <v>20</v>
-      </c>
-      <c r="H83">
-        <v>5</v>
-      </c>
       <c r="I83">
-        <v>215.81</v>
+        <v>199.81</v>
       </c>
       <c r="J83">
-        <v>214.1078033447266</v>
+        <v>201.5414733886719</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3069,127 +3069,127 @@
         <v>0</v>
       </c>
       <c r="B84">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C84">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E84">
+        <v>20</v>
+      </c>
+      <c r="F84">
+        <v>20</v>
+      </c>
+      <c r="G84">
+        <v>28</v>
+      </c>
+      <c r="H84">
         <v>12</v>
       </c>
-      <c r="F84">
-        <v>16</v>
-      </c>
-      <c r="G84">
-        <v>32</v>
-      </c>
-      <c r="H84">
-        <v>8</v>
-      </c>
       <c r="I84">
-        <v>163.61</v>
+        <v>178.26</v>
       </c>
       <c r="J84">
-        <v>186.6832733154297</v>
+        <v>179.0865020751953</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B85">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D85">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F85">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G85">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H85">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I85">
-        <v>195.91</v>
+        <v>203.35</v>
       </c>
       <c r="J85">
-        <v>188.2920379638672</v>
+        <v>214.0617370605469</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B86">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C86">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F86">
         <v>0</v>
       </c>
       <c r="G86">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H86">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="I86">
-        <v>211.02</v>
+        <v>212.29</v>
       </c>
       <c r="J86">
-        <v>200.2413024902344</v>
+        <v>211.0318603515625</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B87">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E87">
+        <v>16</v>
+      </c>
+      <c r="F87">
         <v>12</v>
       </c>
-      <c r="F87">
-        <v>4</v>
-      </c>
       <c r="G87">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="H87">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I87">
-        <v>189.59</v>
+        <v>234.5</v>
       </c>
       <c r="J87">
-        <v>184.5679168701172</v>
+        <v>205.67724609375</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3197,31 +3197,31 @@
         <v>0</v>
       </c>
       <c r="B88">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F88">
         <v>0</v>
       </c>
       <c r="G88">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H88">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I88">
-        <v>201.05</v>
+        <v>206.43</v>
       </c>
       <c r="J88">
-        <v>201.3851013183594</v>
+        <v>207.8435668945312</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3229,7 +3229,7 @@
         <v>0</v>
       </c>
       <c r="B89">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C89">
         <v>5</v>
@@ -3238,86 +3238,86 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F89">
         <v>0</v>
       </c>
       <c r="G89">
-        <v>20</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H89">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I89">
-        <v>234.77</v>
+        <v>196.61</v>
       </c>
       <c r="J89">
-        <v>208.6599731445312</v>
+        <v>182.5894775390625</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B90">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F90">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="H90">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I90">
-        <v>174.17</v>
+        <v>211.67</v>
       </c>
       <c r="J90">
-        <v>190.0064697265625</v>
+        <v>219.5057220458984</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>45.00000000000001</v>
+        <v>5</v>
       </c>
       <c r="F91">
         <v>0</v>
       </c>
       <c r="G91">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I91">
-        <v>168.34</v>
+        <v>213.37</v>
       </c>
       <c r="J91">
-        <v>177.9838104248047</v>
+        <v>205.6536712646484</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3328,28 +3328,476 @@
         <v>12</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E92">
+        <v>12</v>
+      </c>
+      <c r="F92">
         <v>16</v>
       </c>
-      <c r="F92">
-        <v>8</v>
-      </c>
       <c r="G92">
+        <v>36</v>
+      </c>
+      <c r="H92">
+        <v>12</v>
+      </c>
+      <c r="I92">
+        <v>179.43</v>
+      </c>
+      <c r="J92">
+        <v>174.0486755371094</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="B93">
+        <v>25</v>
+      </c>
+      <c r="C93">
+        <v>20</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>10</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>35</v>
+      </c>
+      <c r="H93">
+        <v>10</v>
+      </c>
+      <c r="I93">
+        <v>213.93</v>
+      </c>
+      <c r="J93">
+        <v>205.2559814453125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94">
+        <v>30</v>
+      </c>
+      <c r="C94">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>5</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>45</v>
+      </c>
+      <c r="H94">
+        <v>10</v>
+      </c>
+      <c r="I94">
+        <v>195.4</v>
+      </c>
+      <c r="J94">
+        <v>197.8504028320312</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="B95">
+        <v>40</v>
+      </c>
+      <c r="C95">
+        <v>25</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>10</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>20</v>
+      </c>
+      <c r="H95">
+        <v>5</v>
+      </c>
+      <c r="I95">
+        <v>215.81</v>
+      </c>
+      <c r="J95">
+        <v>210.6429595947266</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="B96">
+        <v>24</v>
+      </c>
+      <c r="C96">
+        <v>8</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>12</v>
+      </c>
+      <c r="F96">
+        <v>16</v>
+      </c>
+      <c r="G96">
+        <v>32</v>
+      </c>
+      <c r="H96">
+        <v>8</v>
+      </c>
+      <c r="I96">
+        <v>163.61</v>
+      </c>
+      <c r="J96">
+        <v>178.7124938964844</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97">
+        <v>4</v>
+      </c>
+      <c r="B97">
+        <v>32</v>
+      </c>
+      <c r="C97">
+        <v>8</v>
+      </c>
+      <c r="D97">
+        <v>4</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+      <c r="F97">
+        <v>20</v>
+      </c>
+      <c r="G97">
+        <v>24</v>
+      </c>
+      <c r="H97">
+        <v>4</v>
+      </c>
+      <c r="I97">
+        <v>195.91</v>
+      </c>
+      <c r="J97">
+        <v>193.2490692138672</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="B98">
+        <v>24</v>
+      </c>
+      <c r="C98">
+        <v>8</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>12</v>
+      </c>
+      <c r="F98">
+        <v>16</v>
+      </c>
+      <c r="G98">
+        <v>32</v>
+      </c>
+      <c r="H98">
+        <v>8</v>
+      </c>
+      <c r="I98">
+        <v>193.2</v>
+      </c>
+      <c r="J98">
+        <v>178.7124938964844</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99">
+        <v>0</v>
+      </c>
+      <c r="B99">
+        <v>20</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>45</v>
+      </c>
+      <c r="H99">
+        <v>25</v>
+      </c>
+      <c r="I99">
+        <v>211.02</v>
+      </c>
+      <c r="J99">
+        <v>205.8189697265625</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100">
+        <v>4</v>
+      </c>
+      <c r="B100">
+        <v>40</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>4</v>
+      </c>
+      <c r="G100">
+        <v>36</v>
+      </c>
+      <c r="H100">
+        <v>4</v>
+      </c>
+      <c r="I100">
+        <v>189.59</v>
+      </c>
+      <c r="J100">
+        <v>192.7719879150391</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>25</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>10</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>50</v>
+      </c>
+      <c r="H101">
+        <v>10</v>
+      </c>
+      <c r="I101">
+        <v>201.05</v>
+      </c>
+      <c r="J101">
+        <v>193.8319549560547</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="B102">
+        <v>40</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>15</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>20</v>
+      </c>
+      <c r="H102">
+        <v>20</v>
+      </c>
+      <c r="I102">
+        <v>234.77</v>
+      </c>
+      <c r="J102">
+        <v>225.5625457763672</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103">
+        <v>0</v>
+      </c>
+      <c r="B103">
+        <v>16</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>4</v>
+      </c>
+      <c r="E103">
+        <v>20</v>
+      </c>
+      <c r="F103">
+        <v>20</v>
+      </c>
+      <c r="G103">
+        <v>28</v>
+      </c>
+      <c r="H103">
+        <v>12</v>
+      </c>
+      <c r="I103">
+        <v>174.17</v>
+      </c>
+      <c r="J103">
+        <v>179.0865020751953</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104">
+        <v>5</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>5</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>45.00000000000001</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>45</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>168.34</v>
+      </c>
+      <c r="J104">
+        <v>171.3014068603516</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105">
+        <v>4</v>
+      </c>
+      <c r="B105">
+        <v>20</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+      <c r="E105">
+        <v>16</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
         <v>52</v>
       </c>
-      <c r="H92">
-        <v>8</v>
-      </c>
-      <c r="I92">
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>195.54</v>
+      </c>
+      <c r="J105">
+        <v>192.5529327392578</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>12</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>16</v>
+      </c>
+      <c r="F106">
+        <v>8</v>
+      </c>
+      <c r="G106">
+        <v>52</v>
+      </c>
+      <c r="H106">
+        <v>8</v>
+      </c>
+      <c r="I106">
         <v>251.53</v>
       </c>
-      <c r="J92">
-        <v>241.5467529296875</v>
+      <c r="J106">
+        <v>227.1830139160156</v>
       </c>
     </row>
   </sheetData>
@@ -3359,7 +3807,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3426,7 +3874,7 @@
         <v>210.99</v>
       </c>
       <c r="J2">
-        <v>194.6778106689453</v>
+        <v>192.5311584472656</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3458,7 +3906,7 @@
         <v>160.84</v>
       </c>
       <c r="J3">
-        <v>185.2934417724609</v>
+        <v>188.2636871337891</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3490,7 +3938,7 @@
         <v>169.12</v>
       </c>
       <c r="J4">
-        <v>185.6759948730469</v>
+        <v>183.9334259033203</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3522,7 +3970,7 @@
         <v>217.16</v>
       </c>
       <c r="J5">
-        <v>195.7407836914062</v>
+        <v>211.0318603515625</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -3554,7 +4002,7 @@
         <v>167.49</v>
       </c>
       <c r="J6">
-        <v>192.7978057861328</v>
+        <v>201.2304840087891</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3586,7 +4034,7 @@
         <v>211.4</v>
       </c>
       <c r="J7">
-        <v>200.2743377685547</v>
+        <v>194.8293304443359</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3618,39 +4066,39 @@
         <v>191.26</v>
       </c>
       <c r="J8">
-        <v>215.1545257568359</v>
+        <v>201.1462860107422</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9">
-        <v>190.61</v>
+        <v>192.46</v>
       </c>
       <c r="J9">
-        <v>203.4894561767578</v>
+        <v>195.6102294921875</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3661,60 +4109,60 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>54.99999999999999</v>
+        <v>70</v>
       </c>
       <c r="H10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>187.6</v>
+        <v>190.61</v>
       </c>
       <c r="J10">
-        <v>204.8750610351562</v>
+        <v>198.7275848388672</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>48</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I11">
-        <v>177.99</v>
+        <v>187.6</v>
       </c>
       <c r="J11">
-        <v>197.2411346435547</v>
+        <v>200.8047790527344</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3722,127 +4170,127 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>168.2</v>
+        <v>177.99</v>
       </c>
       <c r="J12">
-        <v>175.9269409179688</v>
+        <v>192.2540435791016</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>35.00000000000001</v>
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>209.36</v>
+        <v>168.2</v>
       </c>
       <c r="J13">
-        <v>198.8143615722656</v>
+        <v>172.8211364746094</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>35.00000000000001</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="H14">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>196.1</v>
+        <v>209.36</v>
       </c>
       <c r="J14">
-        <v>205.3710632324219</v>
+        <v>182.5234985351562</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="H15">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15">
-        <v>225.55</v>
+        <v>196.1</v>
       </c>
       <c r="J15">
-        <v>225.6396789550781</v>
+        <v>191.7809448242188</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -3850,31 +4298,31 @@
         <v>0</v>
       </c>
       <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
         <v>25</v>
       </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>35</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>25</v>
-      </c>
-      <c r="H16">
-        <v>5</v>
-      </c>
       <c r="I16">
-        <v>182.41</v>
+        <v>225.55</v>
       </c>
       <c r="J16">
-        <v>178.5049285888672</v>
+        <v>225.2430267333984</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3882,63 +4330,63 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H17">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I17">
-        <v>195.94</v>
+        <v>182.41</v>
       </c>
       <c r="J17">
-        <v>197.1261901855469</v>
+        <v>167.4692230224609</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>54.99999999999999</v>
+        <v>40</v>
       </c>
       <c r="H18">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I18">
-        <v>190.35</v>
+        <v>195.94</v>
       </c>
       <c r="J18">
-        <v>186.2116088867188</v>
+        <v>199.2441558837891</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3946,159 +4394,159 @@
         <v>5</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>50</v>
+        <v>54.99999999999999</v>
       </c>
       <c r="H19">
         <v>5</v>
       </c>
       <c r="I19">
-        <v>172.48</v>
+        <v>190.35</v>
       </c>
       <c r="J19">
-        <v>202.6112213134766</v>
+        <v>184.2886047363281</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H20">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I20">
-        <v>221.14</v>
+        <v>172.48</v>
       </c>
       <c r="J20">
-        <v>207.9909362792969</v>
+        <v>225.2126922607422</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B21">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H21">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I21">
-        <v>194.7</v>
+        <v>221.14</v>
       </c>
       <c r="J21">
-        <v>194.3875732421875</v>
+        <v>185.4855804443359</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I22">
-        <v>193.96</v>
+        <v>194.7</v>
       </c>
       <c r="J22">
-        <v>209.2828216552734</v>
+        <v>201.267578125</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
       <c r="G23">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H23">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I23">
-        <v>216.71</v>
+        <v>193.96</v>
       </c>
       <c r="J23">
-        <v>202.5064392089844</v>
+        <v>220.6792602539062</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -4106,31 +4554,31 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H24">
         <v>10</v>
       </c>
       <c r="I24">
-        <v>199.42</v>
+        <v>216.71</v>
       </c>
       <c r="J24">
-        <v>207.5540313720703</v>
+        <v>195.8965301513672</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -4138,95 +4586,159 @@
         <v>0</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C25">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I25">
-        <v>193.04</v>
+        <v>199.42</v>
       </c>
       <c r="J25">
-        <v>167.4161376953125</v>
+        <v>224.2137603759766</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="H26">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>206.62</v>
+        <v>193.04</v>
       </c>
       <c r="J26">
-        <v>204.1601715087891</v>
+        <v>157.3228912353516</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G27">
+        <v>52</v>
+      </c>
+      <c r="H27">
+        <v>24</v>
+      </c>
+      <c r="I27">
+        <v>206.62</v>
+      </c>
+      <c r="J27">
+        <v>193.2413940429688</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>48</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>188.59</v>
+      </c>
+      <c r="J28">
+        <v>176.4345397949219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <v>65</v>
       </c>
-      <c r="H27">
-        <v>5</v>
-      </c>
-      <c r="I27">
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="I29">
         <v>195.66</v>
       </c>
-      <c r="J27">
-        <v>194.6324310302734</v>
+      <c r="J29">
+        <v>201.1484375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>